<commit_message>
toevoeging query releases binnen genre
</commit_message>
<xml_diff>
--- a/mapping.xlsx
+++ b/mapping.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27224"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomruette/Google Drive/data.kunsten.be/visieontwikkeling/Integratienachtmerrie/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Google Drive\Kunstenpunt\Intranet\Data+Docu\Coordinatie\10to1\website en api\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="29000" yWindow="1140" windowWidth="30180" windowHeight="19800" tabRatio="500"/>
+    <workbookView xWindow="28995" yWindow="1140" windowWidth="30180" windowHeight="19800" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="285">
   <si>
     <t>Locatie</t>
   </si>
@@ -881,12 +881,18 @@
   </si>
   <si>
     <t>alle medewerkers aan release</t>
+  </si>
+  <si>
+    <t>releases voor een specifiek genre</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT 'carriers' AS ObjectType, c.ID  FROM carriers c INNER JOIN dblinking gl ON ((gl.ObjectType=5) AND (gl.ObjectID=c.ID) AND (gl.LinkType=11) AND (gl.LinkCategory=28)) INNER JOIN genres g ON gl.LinkID=g.ID WHERE c.Hidden=0 AND (c.Filter&amp;2)=2 AND g.ID=198</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1002,6 +1008,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1272,23 +1281,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="59" customWidth="1"/>
-    <col min="6" max="6" width="35.33203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="35.375" style="2" customWidth="1"/>
     <col min="7" max="7" width="90" customWidth="1"/>
     <col min="8" max="8" width="34.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -1314,7 +1323,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1331,7 +1340,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>24</v>
       </c>
@@ -1342,7 +1351,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>23</v>
       </c>
@@ -1356,7 +1365,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>33</v>
       </c>
@@ -1370,7 +1379,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>34</v>
       </c>
@@ -1384,7 +1393,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>20</v>
       </c>
@@ -1395,7 +1404,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>19</v>
       </c>
@@ -1406,7 +1415,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>42</v>
       </c>
@@ -1417,7 +1426,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>80</v>
       </c>
@@ -1425,7 +1434,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>79</v>
       </c>
@@ -1433,7 +1442,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>18</v>
       </c>
@@ -1447,7 +1456,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>16</v>
       </c>
@@ -1464,7 +1473,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>14</v>
       </c>
@@ -1481,7 +1490,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>12</v>
       </c>
@@ -1498,7 +1507,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>91</v>
       </c>
@@ -1515,7 +1524,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>24</v>
       </c>
@@ -1526,7 +1535,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>92</v>
       </c>
@@ -1537,7 +1546,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -1551,7 +1560,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>23</v>
       </c>
@@ -1562,7 +1571,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>24</v>
       </c>
@@ -1570,7 +1579,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>61</v>
       </c>
@@ -1578,7 +1587,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>62</v>
       </c>
@@ -1586,7 +1595,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>63</v>
       </c>
@@ -1594,7 +1603,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>64</v>
       </c>
@@ -1602,7 +1611,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>65</v>
       </c>
@@ -1610,7 +1619,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>66</v>
       </c>
@@ -1618,7 +1627,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>67</v>
       </c>
@@ -1626,7 +1635,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>68</v>
       </c>
@@ -1634,7 +1643,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>69</v>
       </c>
@@ -1642,7 +1651,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>70</v>
       </c>
@@ -1650,7 +1659,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>71</v>
       </c>
@@ -1658,7 +1667,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>72</v>
       </c>
@@ -1666,7 +1675,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>73</v>
       </c>
@@ -1677,7 +1686,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
         <v>76</v>
       </c>
@@ -1685,7 +1694,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
         <v>75</v>
       </c>
@@ -1693,7 +1702,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>7</v>
       </c>
@@ -1707,7 +1716,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>24</v>
       </c>
@@ -1715,7 +1724,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>122</v>
       </c>
@@ -1723,7 +1732,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>143</v>
       </c>
@@ -1731,7 +1740,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>121</v>
       </c>
@@ -1739,7 +1748,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>142</v>
       </c>
@@ -1747,7 +1756,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>173</v>
       </c>
@@ -1755,7 +1764,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>153</v>
       </c>
@@ -1769,7 +1778,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>24</v>
       </c>
@@ -1777,7 +1786,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>124</v>
       </c>
@@ -1785,7 +1794,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>123</v>
       </c>
@@ -1793,7 +1802,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>155</v>
       </c>
@@ -1801,7 +1810,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>157</v>
       </c>
@@ -1809,7 +1818,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>154</v>
       </c>
@@ -1817,7 +1826,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>7</v>
       </c>
@@ -1831,7 +1840,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>24</v>
       </c>
@@ -1839,7 +1848,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>122</v>
       </c>
@@ -1847,7 +1856,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>143</v>
       </c>
@@ -1855,7 +1864,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>121</v>
       </c>
@@ -1863,7 +1872,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>142</v>
       </c>
@@ -1871,7 +1880,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>150</v>
       </c>
@@ -1879,7 +1888,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>2</v>
       </c>
@@ -1893,7 +1902,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>24</v>
       </c>
@@ -1901,7 +1910,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>121</v>
       </c>
@@ -1909,7 +1918,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>142</v>
       </c>
@@ -1917,7 +1926,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>122</v>
       </c>
@@ -1928,7 +1937,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>143</v>
       </c>
@@ -1936,7 +1945,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
         <v>144</v>
       </c>
@@ -1944,7 +1953,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>145</v>
       </c>
@@ -1952,7 +1961,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>100</v>
       </c>
@@ -1966,7 +1975,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>2</v>
       </c>
@@ -1980,7 +1989,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
         <v>24</v>
       </c>
@@ -1988,7 +1997,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
         <v>121</v>
       </c>
@@ -1996,7 +2005,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
         <v>142</v>
       </c>
@@ -2004,7 +2013,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
         <v>122</v>
       </c>
@@ -2015,7 +2024,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
         <v>143</v>
       </c>
@@ -2023,7 +2032,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
         <v>144</v>
       </c>
@@ -2031,7 +2040,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
         <v>145</v>
       </c>
@@ -2039,7 +2048,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>2</v>
       </c>
@@ -2053,7 +2062,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>24</v>
       </c>
@@ -2061,7 +2070,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
         <v>121</v>
       </c>
@@ -2069,7 +2078,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
         <v>142</v>
       </c>
@@ -2077,7 +2086,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
         <v>122</v>
       </c>
@@ -2088,7 +2097,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
         <v>143</v>
       </c>
@@ -2096,7 +2105,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
         <v>144</v>
       </c>
@@ -2104,7 +2113,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
         <v>145</v>
       </c>
@@ -2112,7 +2121,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>2</v>
       </c>
@@ -2126,7 +2135,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
         <v>24</v>
       </c>
@@ -2134,7 +2143,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
         <v>121</v>
       </c>
@@ -2142,7 +2151,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
         <v>142</v>
       </c>
@@ -2150,7 +2159,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
         <v>122</v>
       </c>
@@ -2161,7 +2170,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
         <v>143</v>
       </c>
@@ -2169,7 +2178,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
         <v>144</v>
       </c>
@@ -2177,7 +2186,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
         <v>145</v>
       </c>
@@ -2185,7 +2194,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>0</v>
       </c>
@@ -2205,7 +2214,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
         <v>24</v>
       </c>
@@ -2216,7 +2225,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>91</v>
       </c>
@@ -2236,7 +2245,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
         <v>24</v>
       </c>
@@ -2247,7 +2256,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
         <v>92</v>
       </c>
@@ -2258,7 +2267,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>91</v>
       </c>
@@ -2278,7 +2287,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
         <v>128</v>
       </c>
@@ -2289,7 +2298,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
         <v>92</v>
       </c>
@@ -2313,23 +2322,23 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>51</v>
       </c>
@@ -2337,7 +2346,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>52</v>
       </c>
@@ -2348,7 +2357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>56</v>
       </c>
@@ -2356,7 +2365,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>53</v>
       </c>
@@ -2367,7 +2376,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>98</v>
       </c>
@@ -2375,7 +2384,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>96</v>
       </c>
@@ -2383,7 +2392,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>97</v>
       </c>
@@ -2391,7 +2400,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>115</v>
       </c>
@@ -2399,7 +2408,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>125</v>
       </c>
@@ -2407,7 +2416,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>126</v>
       </c>
@@ -2415,7 +2424,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>127</v>
       </c>
@@ -2423,7 +2432,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>146</v>
       </c>
@@ -2431,7 +2440,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>55</v>
       </c>
@@ -2439,7 +2448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>57</v>
       </c>
@@ -2447,7 +2456,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>58</v>
       </c>
@@ -2455,7 +2464,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>94</v>
       </c>
@@ -2463,7 +2472,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>95</v>
       </c>
@@ -2471,7 +2480,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>133</v>
       </c>
@@ -2479,7 +2488,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>190</v>
       </c>
@@ -2487,7 +2496,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>191</v>
       </c>
@@ -2495,27 +2504,27 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>189</v>
       </c>
@@ -2527,23 +2536,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B52"/>
+  <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.1640625" customWidth="1"/>
+    <col min="1" max="1" width="37.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>230</v>
       </c>
@@ -2551,7 +2560,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>199</v>
       </c>
@@ -2559,7 +2568,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>257</v>
       </c>
@@ -2567,7 +2576,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>200</v>
       </c>
@@ -2575,7 +2584,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>204</v>
       </c>
@@ -2583,7 +2592,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>231</v>
       </c>
@@ -2591,7 +2600,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>240</v>
       </c>
@@ -2599,7 +2608,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>238</v>
       </c>
@@ -2607,7 +2616,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>241</v>
       </c>
@@ -2615,7 +2624,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>239</v>
       </c>
@@ -2623,7 +2632,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>232</v>
       </c>
@@ -2631,7 +2640,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>233</v>
       </c>
@@ -2639,7 +2648,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>234</v>
       </c>
@@ -2647,7 +2656,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>235</v>
       </c>
@@ -2655,7 +2664,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>201</v>
       </c>
@@ -2663,7 +2672,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>202</v>
       </c>
@@ -2671,7 +2680,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>203</v>
       </c>
@@ -2679,7 +2688,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>227</v>
       </c>
@@ -2687,7 +2696,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>228</v>
       </c>
@@ -2695,7 +2704,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>229</v>
       </c>
@@ -2703,7 +2712,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>281</v>
       </c>
@@ -2711,7 +2720,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>237</v>
       </c>
@@ -2719,7 +2728,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>205</v>
       </c>
@@ -2727,12 +2736,12 @@
         <v>224</v>
       </c>
     </row>
-    <row r="26" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>255</v>
       </c>
@@ -2740,7 +2749,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>256</v>
       </c>
@@ -2748,7 +2757,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>258</v>
       </c>
@@ -2756,7 +2765,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>240</v>
       </c>
@@ -2764,7 +2773,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>238</v>
       </c>
@@ -2772,7 +2781,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>259</v>
       </c>
@@ -2780,7 +2789,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>202</v>
       </c>
@@ -2788,7 +2797,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>203</v>
       </c>
@@ -2796,7 +2805,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>260</v>
       </c>
@@ -2804,7 +2813,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>262</v>
       </c>
@@ -2812,7 +2821,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>261</v>
       </c>
@@ -2820,7 +2829,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>205</v>
       </c>
@@ -2828,12 +2837,12 @@
         <v>253</v>
       </c>
     </row>
-    <row r="40" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>276</v>
       </c>
@@ -2841,7 +2850,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>277</v>
       </c>
@@ -2849,27 +2858,27 @@
         <v>265</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>282</v>
       </c>
@@ -2877,7 +2886,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>236</v>
       </c>
@@ -2885,7 +2894,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>278</v>
       </c>
@@ -2893,12 +2902,12 @@
         <v>272</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>279</v>
       </c>
@@ -2906,12 +2915,20 @@
         <v>274</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>280</v>
       </c>
       <c r="B52" t="s">
         <v>275</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>283</v>
+      </c>
+      <c r="B54" t="s">
+        <v>284</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
beeldmateriaal van release op juiste plaats
</commit_message>
<xml_diff>
--- a/mapping.xlsx
+++ b/mapping.xlsx
@@ -2538,8 +2538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2791,136 +2791,136 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B33" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>203</v>
+        <v>260</v>
       </c>
       <c r="B34" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="B35" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B36" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>261</v>
+        <v>205</v>
       </c>
       <c r="B37" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>205</v>
-      </c>
-      <c r="B38" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="40" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+    <row r="39" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>263</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>276</v>
+      </c>
+      <c r="B40" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B41" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>277</v>
-      </c>
       <c r="B42" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>282</v>
+      </c>
       <c r="B46" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>282</v>
+        <v>236</v>
       </c>
       <c r="B47" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>236</v>
+        <v>278</v>
       </c>
       <c r="B48" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>278</v>
-      </c>
       <c r="B49" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>279</v>
+      </c>
       <c r="B50" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B51" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>280</v>
+        <v>202</v>
       </c>
       <c r="B52" t="s">
-        <v>275</v>
+        <v>248</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update global id strategy
</commit_message>
<xml_diff>
--- a/mapping.xlsx
+++ b/mapping.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28995" yWindow="1140" windowWidth="30180" windowHeight="19800" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="297">
   <si>
     <t>Locatie</t>
   </si>
@@ -316,9 +316,6 @@
     <t>None</t>
   </si>
   <si>
-    <t>datakunstenbe.identitytypes</t>
-  </si>
-  <si>
     <t>datakunstenbe.organisationtypes</t>
   </si>
   <si>
@@ -887,13 +884,52 @@
   </si>
   <si>
     <t>SELECT DISTINCT 'carriers' AS ObjectType, c.ID  FROM carriers c INNER JOIN dblinking gl ON ((gl.ObjectType=5) AND (gl.ObjectID=c.ID) AND (gl.LinkType=11) AND (gl.LinkCategory=28)) INNER JOIN genres g ON gl.LinkID=g.ID WHERE c.Hidden=0 AND (c.Filter&amp;2)=2 AND g.ID=198</t>
+  </si>
+  <si>
+    <t>"1" =&gt; Person,</t>
+  </si>
+  <si>
+    <t>                      "2" =&gt; Organisation,</t>
+  </si>
+  <si>
+    <t>                      "3" =&gt; Venue,</t>
+  </si>
+  <si>
+    <t>                      "4" =&gt; PersonType,</t>
+  </si>
+  <si>
+    <t>                      "5" =&gt; OrganisationType,</t>
+  </si>
+  <si>
+    <t>                      "6" =&gt; Show,</t>
+  </si>
+  <si>
+    <t>                      "7" =&gt; Function,</t>
+  </si>
+  <si>
+    <t>                      "8" =&gt; Genre,</t>
+  </si>
+  <si>
+    <t>                      "9" =&gt; Location,</t>
+  </si>
+  <si>
+    <t>                      "0" =&gt; Production</t>
+  </si>
+  <si>
+    <t>datakunstenbe.persontypes</t>
+  </si>
+  <si>
+    <t>datakunstenbe.shows</t>
+  </si>
+  <si>
+    <t>datakunstenbe.productions</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -924,6 +960,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -968,7 +1010,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -976,6 +1018,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="23">
@@ -1348,7 +1393,7 @@
         <v>35</v>
       </c>
       <c r="G3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1453,7 +1498,7 @@
         <v>37</v>
       </c>
       <c r="G12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1470,7 +1515,7 @@
         <v>46</v>
       </c>
       <c r="G13" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
@@ -1487,7 +1532,7 @@
         <v>49</v>
       </c>
       <c r="G14" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1504,7 +1549,7 @@
         <v>47</v>
       </c>
       <c r="G15" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1518,7 +1563,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G17" t="s">
         <v>88</v>
@@ -1529,7 +1574,7 @@
         <v>24</v>
       </c>
       <c r="E18" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G18" t="s">
         <v>89</v>
@@ -1557,7 +1602,7 @@
         <v>9</v>
       </c>
       <c r="E21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1568,7 +1613,7 @@
         <v>22</v>
       </c>
       <c r="E22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1576,7 +1621,7 @@
         <v>24</v>
       </c>
       <c r="E23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1584,7 +1629,7 @@
         <v>61</v>
       </c>
       <c r="E24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1592,7 +1637,7 @@
         <v>62</v>
       </c>
       <c r="E25" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1600,7 +1645,7 @@
         <v>63</v>
       </c>
       <c r="E26" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1608,7 +1653,7 @@
         <v>64</v>
       </c>
       <c r="E27" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1616,7 +1661,7 @@
         <v>65</v>
       </c>
       <c r="E28" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1624,7 +1669,7 @@
         <v>66</v>
       </c>
       <c r="E29" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1632,7 +1677,7 @@
         <v>67</v>
       </c>
       <c r="E30" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1640,7 +1685,7 @@
         <v>68</v>
       </c>
       <c r="E31" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1648,7 +1693,7 @@
         <v>69</v>
       </c>
       <c r="E32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -1656,7 +1701,7 @@
         <v>70</v>
       </c>
       <c r="E33" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -1664,7 +1709,7 @@
         <v>71</v>
       </c>
       <c r="E34" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -1672,7 +1717,7 @@
         <v>72</v>
       </c>
       <c r="E35" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -1683,7 +1728,7 @@
         <v>74</v>
       </c>
       <c r="E36" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -1691,7 +1736,7 @@
         <v>76</v>
       </c>
       <c r="E37" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -1699,7 +1744,7 @@
         <v>75</v>
       </c>
       <c r="E38" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -1710,10 +1755,10 @@
         <v>26</v>
       </c>
       <c r="D40" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G40" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -1721,52 +1766,52 @@
         <v>24</v>
       </c>
       <c r="G41" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G42" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G43" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G44" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G45" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G46" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B48" t="s">
         <v>26</v>
@@ -1775,7 +1820,7 @@
         <v>8</v>
       </c>
       <c r="G48" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -1783,47 +1828,47 @@
         <v>24</v>
       </c>
       <c r="G49" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G50" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G51" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
+        <v>154</v>
+      </c>
+      <c r="G52" t="s">
         <v>155</v>
-      </c>
-      <c r="G52" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
+        <v>156</v>
+      </c>
+      <c r="G53" t="s">
         <v>157</v>
-      </c>
-      <c r="G53" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G54" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -1837,7 +1882,7 @@
         <v>6</v>
       </c>
       <c r="G56" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -1845,47 +1890,47 @@
         <v>24</v>
       </c>
       <c r="G57" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G58" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G59" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G60" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G61" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G62" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -1899,7 +1944,7 @@
         <v>5</v>
       </c>
       <c r="G64" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
@@ -1907,72 +1952,72 @@
         <v>24</v>
       </c>
       <c r="G65" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G66" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G67" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G68" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H68" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G69" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G70" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G71" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B73" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D73" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G73" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
@@ -1986,7 +2031,7 @@
         <v>4</v>
       </c>
       <c r="G75" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
@@ -1994,58 +2039,58 @@
         <v>24</v>
       </c>
       <c r="G76" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G77" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G78" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G79" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H79" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G80" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G81" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G82" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
@@ -2059,7 +2104,7 @@
         <v>3</v>
       </c>
       <c r="G84" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
@@ -2067,58 +2112,58 @@
         <v>24</v>
       </c>
       <c r="G85" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G86" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G87" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G88" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H88" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G89" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G90" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G91" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
@@ -2132,7 +2177,7 @@
         <v>1</v>
       </c>
       <c r="G93" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
@@ -2140,58 +2185,58 @@
         <v>24</v>
       </c>
       <c r="G94" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G95" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G96" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G97" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H97" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G98" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G99" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G100" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
@@ -2205,13 +2250,13 @@
         <v>0</v>
       </c>
       <c r="E102" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G102" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H102" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
@@ -2219,10 +2264,10 @@
         <v>24</v>
       </c>
       <c r="E103" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G103" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
@@ -2236,13 +2281,13 @@
         <v>60</v>
       </c>
       <c r="E105" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F105" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="G105" t="s">
         <v>137</v>
-      </c>
-      <c r="G105" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
@@ -2250,10 +2295,10 @@
         <v>24</v>
       </c>
       <c r="E106" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G106" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
@@ -2275,27 +2320,27 @@
         <v>26</v>
       </c>
       <c r="D109" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E109" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G109" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E110" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G110" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
@@ -2316,10 +2361,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2330,12 +2375,12 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2370,7 +2415,7 @@
         <v>53</v>
       </c>
       <c r="B9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -2378,7 +2423,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -2386,7 +2431,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C11">
         <v>3</v>
@@ -2394,7 +2439,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C12">
         <v>4</v>
@@ -2402,7 +2447,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C13">
         <v>5</v>
@@ -2410,7 +2455,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C14">
         <v>6</v>
@@ -2418,7 +2463,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C15">
         <v>7</v>
@@ -2426,21 +2471,21 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C16">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C17">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>55</v>
       </c>
@@ -2448,7 +2493,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>57</v>
       </c>
@@ -2456,7 +2501,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>58</v>
       </c>
@@ -2464,73 +2509,130 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>94</v>
+        <v>294</v>
       </c>
       <c r="C22">
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C23">
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>133</v>
+        <v>295</v>
       </c>
       <c r="C24">
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>190</v>
+        <v>132</v>
       </c>
       <c r="C25">
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C26">
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>190</v>
+      </c>
+      <c r="C27">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>296</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>184</v>
+      </c>
+      <c r="L29" s="4" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="57" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="L30" s="4" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="L31" s="4" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="57" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="L32" s="4" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="57" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>189</v>
+      <c r="L33" s="4" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="L34" s="4" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="L35" s="4" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="L36" s="4" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="L37" s="4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="L38" s="4" t="s">
+        <v>293</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2538,7 +2640,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
@@ -2549,386 +2651,386 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B10" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B11" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B12" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B13" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B14" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B15" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B16" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B17" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B18" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B19" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B20" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B21" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B23" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B24" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="26" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B27" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B28" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B29" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B30" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B31" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B32" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B33" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B34" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B35" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B36" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B37" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="39" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B40" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B41" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B46" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B47" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B48" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B50" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B51" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B52" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>282</v>
+      </c>
+      <c r="B54" t="s">
         <v>283</v>
-      </c>
-      <c r="B54" t="s">
-        <v>284</v>
       </c>
     </row>
   </sheetData>

</xml_diff>